<commit_message>
KnightTraverse function in Knightmove.h DONE
with backtracking
</commit_message>
<xml_diff>
--- a/TimeScheme.xlsx
+++ b/TimeScheme.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Start</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>Damn!!!</t>
   </si>
   <si>
     <t>Good time</t>
@@ -463,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -519,7 +516,7 @@
         <v>41294.666956018518</v>
       </c>
       <c r="C2" s="3">
-        <v>41293.680844907409</v>
+        <v>41294.680844907409</v>
       </c>
       <c r="D2" s="4">
         <f>HOUR(C2)+MINUTE(C2)/60-(HOUR(B2)+MINUTE(B2)/60)</f>
@@ -529,11 +526,11 @@
         <v>0.5</v>
       </c>
       <c r="F2">
-        <f>E2*$D$14</f>
+        <f>E2*$D$17</f>
         <v>15.56016597510374</v>
       </c>
       <c r="G2">
-        <f>D2*$D$14</f>
+        <f>D2*$D$17</f>
         <v>10.373443983402456</v>
       </c>
       <c r="H2">
@@ -545,7 +542,7 @@
         <v>20.746887966805023</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -566,11 +563,11 @@
         <v>0.8</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F10" si="1">E3*$D$14</f>
+        <f t="shared" ref="F3:F10" si="1">E3*$D$17</f>
         <v>24.896265560165986</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G10" si="2">D3*$D$14</f>
+        <f t="shared" ref="G3:G10" si="2">D3*$D$17</f>
         <v>16.597510373443932</v>
       </c>
       <c r="H3">
@@ -582,7 +579,7 @@
         <v>33.195020746888041</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -619,44 +616,56 @@
         <v>15.041493775933553</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B5" s="3">
+        <v>41294.736635879628</v>
+      </c>
+      <c r="C5" s="3">
+        <v>41294.740485416667</v>
+      </c>
       <c r="D5" s="4">
         <f>HOUR(C5)+MINUTE(C5)/60-(HOUR(B5)+MINUTE(B5)/60)</f>
-        <v>0</v>
+        <v>9.9999999999997868E-2</v>
       </c>
       <c r="E5">
         <v>0.1</v>
       </c>
       <c r="F5">
-        <f>E5*$D$14</f>
+        <f>E5*$D$17</f>
         <v>3.1120331950207483</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.1120331950206817</v>
       </c>
       <c r="H5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.1120331950207483</v>
       </c>
       <c r="I5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.1120331950208149</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B6" s="3">
+        <v>41294.740485416667</v>
+      </c>
+      <c r="C6" s="3">
+        <v>41294.744398148148</v>
+      </c>
       <c r="D6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333335702E-2</v>
       </c>
       <c r="E6">
         <v>0.1</v>
@@ -667,43 +676,52 @@
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.5933609958506971</v>
       </c>
       <c r="H6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.1120331950207483</v>
       </c>
       <c r="I6">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.6307053941907994</v>
+      </c>
+      <c r="J6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B7" s="3">
+        <v>41294.815879629627</v>
+      </c>
+      <c r="C7" s="3">
+        <v>41294.947791319442</v>
+      </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.1666666666666679</v>
       </c>
       <c r="E7">
         <v>2.17</v>
       </c>
       <c r="F7">
-        <f>E7*$D$14</f>
+        <f>E7*$D$17</f>
         <v>67.531120331950234</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>98.547717842323721</v>
       </c>
       <c r="H7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>67.531120331950234</v>
       </c>
       <c r="I7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>36.514522821576747</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -718,7 +736,7 @@
         <v>0.6</v>
       </c>
       <c r="F8">
-        <f>E8*$D$14</f>
+        <f>E8*$D$17</f>
         <v>18.672199170124486</v>
       </c>
       <c r="G8">
@@ -774,7 +792,7 @@
         <v>0.1</v>
       </c>
       <c r="F10">
-        <f>E10*$D$14</f>
+        <f>E10*$D$17</f>
         <v>3.1120331950207483</v>
       </c>
       <c r="G10">
@@ -795,7 +813,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="3">
-        <v>41293.680844907409</v>
+        <v>41294.680844907409</v>
       </c>
       <c r="C11" s="3">
         <v>41294.705441319442</v>
@@ -804,14 +822,11 @@
         <f t="shared" ref="D11" si="5">HOUR(C11)+MINUTE(C11)/60-(HOUR(B11)+MINUTE(B11)/60)</f>
         <v>0.5833333333333357</v>
       </c>
-      <c r="E11">
-        <v>0.2</v>
-      </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11" si="6">D11*$D$14</f>
+        <f t="shared" ref="G11" si="6">D11*$D$17</f>
         <v>18.153526970954438</v>
       </c>
       <c r="H11">
@@ -822,44 +837,113 @@
         <f t="shared" ref="I11" si="8">IF(G11&gt;0,H11+H11-G11,0)</f>
         <v>-18.153526970954438</v>
       </c>
-      <c r="J11" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="H12" s="6">
-        <f>SUM(H2:H11)</f>
-        <v>51.348547717842344</v>
-      </c>
-      <c r="I12" s="5">
-        <f>SUM(I2:I11)</f>
-        <v>50.829875518672189</v>
+      <c r="A12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4">
+        <f t="shared" ref="D12:D14" si="9">HOUR(C12)+MINUTE(C12)/60-(HOUR(B12)+MINUTE(B12)/60)</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G14" si="10">D12*$D$17</f>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ref="H12:H14" si="11">IF(G12&gt;0,F12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:I14" si="12">IF(G12&gt;0,H12+H12-G12,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="B13" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="H15" s="6">
+        <f>SUM(H2:H14)</f>
+        <v>125.10373443983408</v>
+      </c>
+      <c r="I15" s="5">
+        <f>SUM(I2:I14)</f>
+        <v>94.087136929460542</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B17">
         <v>150</v>
       </c>
-      <c r="C14">
+      <c r="C17">
         <f>SUM(E2:E10)</f>
         <v>4.8199999999999985</v>
       </c>
-      <c r="D14">
-        <f>B14/C14</f>
+      <c r="D17">
+        <f>B17/C17</f>
         <v>31.120331950207479</v>
       </c>
     </row>

</xml_diff>